<commit_message>
Correcao de bugs do banco quando ele fica travado
</commit_message>
<xml_diff>
--- a/excel_sistema.xlsx
+++ b/excel_sistema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="22995" windowHeight="9975" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="22995" windowHeight="9975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CursoAno" sheetId="1" r:id="rId1"/>
@@ -1222,7 +1222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1360,15 +1360,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1681,7 +1682,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,7 +2119,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U218"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2669,22 +2672,22 @@
         <v>4</v>
       </c>
       <c r="D28" s="18"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="45"/>
       <c r="H28" s="22"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
-      <c r="N28" s="43"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="18"/>
-      <c r="P28" s="43"/>
+      <c r="P28" s="46"/>
       <c r="Q28" s="18"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="44"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="45"/>
       <c r="U28" s="22"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -2698,22 +2701,22 @@
         <v>4</v>
       </c>
       <c r="D29" s="19"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
       <c r="H29" s="21"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
-      <c r="N29" s="44"/>
+      <c r="N29" s="45"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="44"/>
+      <c r="P29" s="45"/>
       <c r="Q29" s="19"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="44"/>
-      <c r="T29" s="44"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
       <c r="U29" s="21"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -6973,113 +6976,113 @@
     </row>
     <row r="197" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B197" s="18"/>
-      <c r="C197" s="43"/>
+      <c r="C197" s="46"/>
       <c r="D197" s="18"/>
-      <c r="E197" s="43"/>
-      <c r="F197" s="43"/>
-      <c r="G197" s="44"/>
+      <c r="E197" s="46"/>
+      <c r="F197" s="46"/>
+      <c r="G197" s="45"/>
       <c r="H197" s="17"/>
       <c r="I197" s="14"/>
       <c r="J197" s="14"/>
       <c r="K197" s="14"/>
       <c r="L197" s="14"/>
       <c r="M197" s="14"/>
-      <c r="N197" s="43"/>
+      <c r="N197" s="46"/>
       <c r="O197" s="18"/>
-      <c r="P197" s="43"/>
+      <c r="P197" s="46"/>
       <c r="Q197" s="18"/>
-      <c r="R197" s="43"/>
-      <c r="S197" s="43"/>
-      <c r="T197" s="44"/>
+      <c r="R197" s="46"/>
+      <c r="S197" s="46"/>
+      <c r="T197" s="45"/>
       <c r="U197" s="17"/>
     </row>
     <row r="198" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B198" s="19"/>
-      <c r="C198" s="44"/>
+      <c r="C198" s="45"/>
       <c r="D198" s="19"/>
-      <c r="E198" s="44"/>
-      <c r="F198" s="44"/>
-      <c r="G198" s="44"/>
+      <c r="E198" s="45"/>
+      <c r="F198" s="45"/>
+      <c r="G198" s="45"/>
       <c r="H198" s="17"/>
       <c r="I198" s="14"/>
       <c r="J198" s="14"/>
       <c r="K198" s="14"/>
       <c r="L198" s="14"/>
       <c r="M198" s="14"/>
-      <c r="N198" s="44"/>
+      <c r="N198" s="45"/>
       <c r="O198" s="19"/>
-      <c r="P198" s="44"/>
+      <c r="P198" s="45"/>
       <c r="Q198" s="19"/>
-      <c r="R198" s="44"/>
-      <c r="S198" s="44"/>
-      <c r="T198" s="44"/>
+      <c r="R198" s="45"/>
+      <c r="S198" s="45"/>
+      <c r="T198" s="45"/>
       <c r="U198" s="17"/>
     </row>
     <row r="199" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B199" s="24"/>
-      <c r="C199" s="43"/>
+      <c r="C199" s="46"/>
       <c r="D199" s="18"/>
-      <c r="E199" s="43"/>
-      <c r="F199" s="43"/>
-      <c r="G199" s="44"/>
-      <c r="H199" s="45"/>
+      <c r="E199" s="46"/>
+      <c r="F199" s="46"/>
+      <c r="G199" s="45"/>
+      <c r="H199" s="44"/>
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
       <c r="K199" s="14"/>
       <c r="L199" s="14"/>
       <c r="M199" s="14"/>
-      <c r="N199" s="46"/>
+      <c r="N199" s="47"/>
       <c r="O199" s="24"/>
-      <c r="P199" s="43"/>
+      <c r="P199" s="46"/>
       <c r="Q199" s="18"/>
-      <c r="R199" s="43"/>
-      <c r="S199" s="43"/>
-      <c r="T199" s="44"/>
-      <c r="U199" s="45"/>
+      <c r="R199" s="46"/>
+      <c r="S199" s="46"/>
+      <c r="T199" s="45"/>
+      <c r="U199" s="44"/>
     </row>
     <row r="200" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B200" s="25"/>
-      <c r="C200" s="44"/>
+      <c r="C200" s="45"/>
       <c r="D200" s="19"/>
-      <c r="E200" s="44"/>
-      <c r="F200" s="44"/>
-      <c r="G200" s="44"/>
-      <c r="H200" s="44"/>
+      <c r="E200" s="45"/>
+      <c r="F200" s="45"/>
+      <c r="G200" s="45"/>
+      <c r="H200" s="45"/>
       <c r="I200" s="14"/>
       <c r="J200" s="14"/>
       <c r="K200" s="14"/>
       <c r="L200" s="14"/>
       <c r="M200" s="14"/>
-      <c r="N200" s="47"/>
+      <c r="N200" s="48"/>
       <c r="O200" s="25"/>
-      <c r="P200" s="44"/>
+      <c r="P200" s="45"/>
       <c r="Q200" s="19"/>
-      <c r="R200" s="44"/>
-      <c r="S200" s="44"/>
-      <c r="T200" s="44"/>
-      <c r="U200" s="44"/>
+      <c r="R200" s="45"/>
+      <c r="S200" s="45"/>
+      <c r="T200" s="45"/>
+      <c r="U200" s="45"/>
     </row>
     <row r="201" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B201" s="25"/>
-      <c r="C201" s="44"/>
+      <c r="C201" s="45"/>
       <c r="D201" s="19"/>
-      <c r="E201" s="44"/>
-      <c r="F201" s="44"/>
-      <c r="G201" s="44"/>
-      <c r="H201" s="44"/>
+      <c r="E201" s="45"/>
+      <c r="F201" s="45"/>
+      <c r="G201" s="45"/>
+      <c r="H201" s="45"/>
       <c r="I201" s="14"/>
       <c r="J201" s="14"/>
       <c r="K201" s="14"/>
       <c r="L201" s="14"/>
       <c r="M201" s="14"/>
-      <c r="N201" s="47"/>
+      <c r="N201" s="48"/>
       <c r="O201" s="25"/>
-      <c r="P201" s="44"/>
+      <c r="P201" s="45"/>
       <c r="Q201" s="19"/>
-      <c r="R201" s="44"/>
-      <c r="S201" s="44"/>
-      <c r="T201" s="44"/>
-      <c r="U201" s="44"/>
+      <c r="R201" s="45"/>
+      <c r="S201" s="45"/>
+      <c r="T201" s="45"/>
+      <c r="U201" s="45"/>
     </row>
     <row r="202" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B202" s="12"/>
@@ -7457,23 +7460,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="U199:U201"/>
-    <mergeCell ref="N197:N198"/>
-    <mergeCell ref="P197:P198"/>
-    <mergeCell ref="R197:R198"/>
-    <mergeCell ref="S197:S198"/>
-    <mergeCell ref="T197:T198"/>
-    <mergeCell ref="N199:N201"/>
-    <mergeCell ref="P199:P201"/>
-    <mergeCell ref="R199:R201"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="E197:E198"/>
-    <mergeCell ref="F197:F198"/>
-    <mergeCell ref="G197:G198"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="E199:E201"/>
-    <mergeCell ref="F199:F201"/>
-    <mergeCell ref="G199:G201"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
@@ -7485,6 +7471,23 @@
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
     <mergeCell ref="T199:T201"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="E197:E198"/>
+    <mergeCell ref="F197:F198"/>
+    <mergeCell ref="G197:G198"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="E199:E201"/>
+    <mergeCell ref="F199:F201"/>
+    <mergeCell ref="G199:G201"/>
+    <mergeCell ref="U199:U201"/>
+    <mergeCell ref="N197:N198"/>
+    <mergeCell ref="P197:P198"/>
+    <mergeCell ref="R197:R198"/>
+    <mergeCell ref="S197:S198"/>
+    <mergeCell ref="T197:T198"/>
+    <mergeCell ref="N199:N201"/>
+    <mergeCell ref="P199:P201"/>
+    <mergeCell ref="R199:R201"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
@@ -7495,8 +7498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7575,7 +7578,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>0.72222222222222221</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="B10" s="4">
         <v>0.75</v>
@@ -7583,15 +7586,13 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.75</v>
-      </c>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>0.68055555555555547</v>
+        <v>0.75</v>
       </c>
       <c r="B12" s="4">
         <v>0.79166666666666663</v>
@@ -7599,46 +7600,42 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="B13" s="4">
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="B14" s="4">
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="B15" s="4">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="B16" s="4">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.91666666666666663</v>
-      </c>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7646,8 +7643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel com fonte negrita, centralizado e com o nome da sala em uma celula maior. Tem um bug que o tomcat reclama da Celula nao ser serializable.
</commit_message>
<xml_diff>
--- a/excel_sistema.xlsx
+++ b/excel_sistema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="22995" windowHeight="9975" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="22995" windowHeight="9975" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CursoAno" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="376">
   <si>
     <t>Sigla</t>
   </si>
@@ -1361,15 +1361,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1681,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U218"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,8 +2672,8 @@
         <v>4</v>
       </c>
       <c r="D28" s="18"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
       <c r="G28" s="45"/>
       <c r="H28" s="22"/>
       <c r="I28" s="14"/>
@@ -2681,12 +2681,12 @@
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
-      <c r="N28" s="46"/>
+      <c r="N28" s="44"/>
       <c r="O28" s="18"/>
-      <c r="P28" s="46"/>
+      <c r="P28" s="44"/>
       <c r="Q28" s="18"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
       <c r="T28" s="45"/>
       <c r="U28" s="22"/>
     </row>
@@ -6976,10 +6976,10 @@
     </row>
     <row r="197" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B197" s="18"/>
-      <c r="C197" s="46"/>
+      <c r="C197" s="44"/>
       <c r="D197" s="18"/>
-      <c r="E197" s="46"/>
-      <c r="F197" s="46"/>
+      <c r="E197" s="44"/>
+      <c r="F197" s="44"/>
       <c r="G197" s="45"/>
       <c r="H197" s="17"/>
       <c r="I197" s="14"/>
@@ -6987,12 +6987,12 @@
       <c r="K197" s="14"/>
       <c r="L197" s="14"/>
       <c r="M197" s="14"/>
-      <c r="N197" s="46"/>
+      <c r="N197" s="44"/>
       <c r="O197" s="18"/>
-      <c r="P197" s="46"/>
+      <c r="P197" s="44"/>
       <c r="Q197" s="18"/>
-      <c r="R197" s="46"/>
-      <c r="S197" s="46"/>
+      <c r="R197" s="44"/>
+      <c r="S197" s="44"/>
       <c r="T197" s="45"/>
       <c r="U197" s="17"/>
     </row>
@@ -7020,12 +7020,12 @@
     </row>
     <row r="199" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B199" s="24"/>
-      <c r="C199" s="46"/>
+      <c r="C199" s="44"/>
       <c r="D199" s="18"/>
-      <c r="E199" s="46"/>
-      <c r="F199" s="46"/>
+      <c r="E199" s="44"/>
+      <c r="F199" s="44"/>
       <c r="G199" s="45"/>
-      <c r="H199" s="44"/>
+      <c r="H199" s="46"/>
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
       <c r="K199" s="14"/>
@@ -7033,12 +7033,12 @@
       <c r="M199" s="14"/>
       <c r="N199" s="47"/>
       <c r="O199" s="24"/>
-      <c r="P199" s="46"/>
+      <c r="P199" s="44"/>
       <c r="Q199" s="18"/>
-      <c r="R199" s="46"/>
-      <c r="S199" s="46"/>
+      <c r="R199" s="44"/>
+      <c r="S199" s="44"/>
       <c r="T199" s="45"/>
-      <c r="U199" s="44"/>
+      <c r="U199" s="46"/>
     </row>
     <row r="200" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B200" s="25"/>
@@ -7460,6 +7460,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="U199:U201"/>
+    <mergeCell ref="N197:N198"/>
+    <mergeCell ref="P197:P198"/>
+    <mergeCell ref="R197:R198"/>
+    <mergeCell ref="S197:S198"/>
+    <mergeCell ref="T197:T198"/>
+    <mergeCell ref="N199:N201"/>
+    <mergeCell ref="P199:P201"/>
+    <mergeCell ref="R199:R201"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="E197:E198"/>
+    <mergeCell ref="F197:F198"/>
+    <mergeCell ref="G197:G198"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="E199:E201"/>
+    <mergeCell ref="F199:F201"/>
+    <mergeCell ref="G199:G201"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
@@ -7471,23 +7488,6 @@
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
     <mergeCell ref="T199:T201"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="E197:E198"/>
-    <mergeCell ref="F197:F198"/>
-    <mergeCell ref="G197:G198"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="E199:E201"/>
-    <mergeCell ref="F199:F201"/>
-    <mergeCell ref="G199:G201"/>
-    <mergeCell ref="U199:U201"/>
-    <mergeCell ref="N197:N198"/>
-    <mergeCell ref="P197:P198"/>
-    <mergeCell ref="R197:R198"/>
-    <mergeCell ref="S197:S198"/>
-    <mergeCell ref="T197:T198"/>
-    <mergeCell ref="N199:N201"/>
-    <mergeCell ref="P199:P201"/>
-    <mergeCell ref="R199:R201"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
@@ -7498,8 +7498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7641,10 +7641,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140:XFD140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8181,177 +8181,177 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C30" s="9">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>148</v>
       </c>
       <c r="C31" s="9">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>310</v>
+        <v>79</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="9">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>300</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="2">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="9">
+        <v>64</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>320</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>151</v>
       </c>
       <c r="C34" s="9">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="2">
         <v>14</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C35" s="9">
-        <v>73</v>
-      </c>
       <c r="D35" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>321</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C36" s="2">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="9">
+        <v>6</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E36" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C37" s="9">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>70</v>
+        <v>310</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>74</v>
+        <v>311</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C38" s="9">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>310</v>
+        <v>72</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C39" s="9">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>72</v>
+        <v>302</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>323</v>
+        <v>76</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -8360,61 +8360,59 @@
         <v>5</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C40" s="9">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C41" s="9">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>163</v>
+        <v>354</v>
       </c>
       <c r="C42" s="9">
-        <v>1</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>76</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>354</v>
+      <c r="B43" s="10" t="s">
+        <v>355</v>
       </c>
       <c r="C43" s="9">
         <v>25</v>
@@ -8427,71 +8425,73 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>355</v>
+        <v>37</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C44" s="9">
-        <v>25</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C45" s="9">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>314</v>
+        <v>324</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>325</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C46" s="9">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>327</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C47" s="9">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -8500,28 +8500,28 @@
         <v>22</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C48" s="9">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C49" s="9">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>324</v>
@@ -8536,16 +8536,16 @@
         <v>23</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C50" s="9">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -8554,52 +8554,52 @@
         <v>23</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C51" s="9">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C52" s="9">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C53" s="9">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -8608,52 +8608,52 @@
         <v>23</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C54" s="9">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C55" s="9">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C56" s="9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -8662,80 +8662,80 @@
         <v>24</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C57" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C58" s="9">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="2">
+        <v>30</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>327</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C59" s="2">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="9">
+        <v>21</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>331</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C60" s="9">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>329</v>
+        <v>305</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>304</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>197</v>
       </c>
       <c r="C61" s="9">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>305</v>
@@ -8746,14 +8746,14 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>13</v>
+      <c r="A62" t="s">
+        <v>359</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>197</v>
       </c>
       <c r="C62" s="9">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>305</v>
@@ -8764,32 +8764,32 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>359</v>
+      <c r="A63" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C63" s="9">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>199</v>
       </c>
       <c r="C64" s="9">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>310</v>
@@ -8800,14 +8800,14 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>13</v>
+      <c r="A65" t="s">
+        <v>359</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>199</v>
       </c>
       <c r="C65" s="9">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>310</v>
@@ -8818,50 +8818,50 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>359</v>
+      <c r="A66" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>199</v>
       </c>
       <c r="C66" s="9">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>310</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>311</v>
+        <v>74</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C67" s="9">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>74</v>
+        <v>304</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>201</v>
       </c>
       <c r="C68" s="9">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>305</v>
@@ -8873,19 +8873,19 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C69" s="9">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>305</v>
+        <v>81</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="F69" s="1"/>
     </row>
@@ -8893,82 +8893,80 @@
       <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="C70" s="9">
-        <v>48</v>
+      <c r="B70" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" s="2">
+        <v>19</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>308</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C71" s="2">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C71" s="9">
+        <v>52</v>
       </c>
       <c r="D71" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C72" s="9">
-        <v>52</v>
+        <v>10</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" s="2">
+        <v>15</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>309</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>209</v>
       </c>
       <c r="C73" s="2">
-        <v>15</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>311</v>
+        <v>38</v>
+      </c>
+      <c r="D73" s="35" t="s">
+        <v>80</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C74" s="2">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="C74" s="9">
+        <v>73</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -8978,7 +8976,7 @@
         <v>12</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C75" s="9">
         <v>73</v>
@@ -8991,82 +8989,82 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>373</v>
+        <v>212</v>
       </c>
       <c r="C76" s="9">
-        <v>73</v>
-      </c>
-      <c r="D76" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="E76" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C77" s="9">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C77" s="2">
+        <v>19</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>75</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>11</v>
+        <v>361</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>214</v>
       </c>
       <c r="C78" s="2">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>214</v>
       </c>
       <c r="C79" s="2">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>362</v>
+        <v>12</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C80" s="2">
         <v>24</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -9076,49 +9074,49 @@
         <v>12</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C81" s="2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C82" s="2">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C82" s="9">
+        <v>22</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="E82" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>304</v>
+      </c>
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C83" s="9">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C83" s="2">
+        <v>12</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>304</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -9126,13 +9124,13 @@
         <v>12</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C84" s="2">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -9142,31 +9140,33 @@
         <v>12</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C85" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C86" s="2">
-        <v>49</v>
+        <v>35</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C86" s="9">
+        <v>39</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="E86" s="1"/>
+        <v>318</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -9174,35 +9174,33 @@
         <v>35</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C87" s="9">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="C88" s="9">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C88" s="2">
+        <v>8</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -9210,63 +9208,63 @@
         <v>39</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C89" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C90" s="2">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C90" s="9">
+        <v>30</v>
       </c>
       <c r="D90" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="C91" s="9">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C91" s="2">
+        <v>6</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C92" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -9276,309 +9274,313 @@
         <v>39</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C93" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C94" s="2">
-        <v>12</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E94" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C94" s="9">
+        <v>30</v>
+      </c>
+      <c r="D94" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>329</v>
+      </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="C95" s="9">
-        <v>30</v>
-      </c>
-      <c r="D95" s="35" t="s">
-        <v>314</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>329</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C95" s="2">
+        <v>12</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C96" s="2">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C96" s="9">
+        <v>9</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="E96" s="1"/>
+        <v>310</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>341</v>
+      </c>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C97" s="2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>10</v>
+        <v>361</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C98" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C99" s="2">
         <v>11</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C99" s="9">
-        <v>9</v>
-      </c>
       <c r="D99" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>341</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C100" s="9">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C100" s="2">
+        <v>46</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>311</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>8</v>
+        <v>365</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>246</v>
       </c>
       <c r="C101" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>246</v>
       </c>
       <c r="C102" s="2">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>300</v>
+        <v>76</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>246</v>
       </c>
       <c r="C103" s="2">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>246</v>
       </c>
       <c r="C104" s="2">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>246</v>
       </c>
       <c r="C105" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>75</v>
+        <v>342</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>366</v>
+        <v>12</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C106" s="2">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>76</v>
+        <v>343</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>359</v>
+        <v>16</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C107" s="2">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C108" s="2">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C108" s="9">
+        <v>13</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E108" s="1"/>
+        <v>310</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>369</v>
+        <v>12</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C109" s="2">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C110" s="2">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" s="9">
+        <v>22</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="E110" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C111" s="2">
-        <v>41</v>
+        <v>14</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C111" s="9">
+        <v>50</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="E111" s="1"/>
+        <v>311</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>304</v>
+      </c>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -9586,216 +9588,214 @@
         <v>10</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C112" s="9">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>310</v>
+        <v>79</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C113" s="2">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C113" s="9">
+        <v>15</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="E113" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>311</v>
+      </c>
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C114" s="9">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D114" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E114" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E114" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="C115" s="9">
-        <v>50</v>
+        <v>11</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" s="2">
+        <v>36</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>304</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C116" s="9">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C116" s="2">
+        <v>21</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>300</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C117" s="9">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C117" s="2">
+        <v>6</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>302</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="C118" s="9">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C118" s="2">
+        <v>8</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>311</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C119" s="9">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>80</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C120" s="2">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C120" s="9">
+        <v>31</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="E120" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C121" s="2">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C122" s="2">
-        <v>6</v>
+        <v>37</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C122" s="9">
+        <v>28</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="E122" s="1"/>
+        <v>324</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>329</v>
+      </c>
       <c r="F122" s="1"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C123" s="2">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C123" s="9">
+        <v>25</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="E123" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="C124" s="9">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C124" s="2">
+        <v>12</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>313</v>
@@ -9805,47 +9805,45 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="C125" s="9">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C125" s="2">
+        <v>18</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E125" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C126" s="2">
-        <v>3</v>
+        <v>38</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C126" s="9">
+        <v>27</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="C127" s="9">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>324</v>
@@ -9857,34 +9855,32 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B128" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="C128" s="9">
         <v>37</v>
       </c>
-      <c r="B128" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="C128" s="9">
-        <v>25</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E128" s="6" t="s">
-        <v>316</v>
-      </c>
+      <c r="D128" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="E128" s="1"/>
       <c r="F128" s="1"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C129" s="2">
-        <v>12</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>313</v>
+        <v>39</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C129" s="9">
+        <v>37</v>
+      </c>
+      <c r="D129" s="35" t="s">
+        <v>348</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -9893,287 +9889,189 @@
       <c r="A130" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C130" s="2">
-        <v>18</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>329</v>
+      <c r="B130" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C130" s="9">
+        <v>37</v>
+      </c>
+      <c r="D130" s="35" t="s">
+        <v>348</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="C131" s="9">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C131" s="2">
+        <v>9</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>314</v>
+        <v>349</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B132" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C132" s="9">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C132" s="5">
+        <v>11</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="E132" s="6" t="s">
-        <v>329</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B133" s="33" t="s">
-        <v>358</v>
-      </c>
-      <c r="C133" s="9">
-        <v>37</v>
-      </c>
-      <c r="D133" s="35" t="s">
-        <v>348</v>
+        <v>18</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C133" s="5">
+        <v>22</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>350</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>357</v>
+        <v>5</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>283</v>
       </c>
       <c r="C134" s="9">
-        <v>37</v>
-      </c>
-      <c r="D134" s="35" t="s">
-        <v>348</v>
-      </c>
-      <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>356</v>
+        <v>8</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="C135" s="9">
-        <v>37</v>
-      </c>
-      <c r="D135" s="35" t="s">
-        <v>348</v>
-      </c>
-      <c r="E135" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C136" s="2">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C136" s="9">
+        <v>76</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="E136" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B137" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C137" s="5">
-        <v>11</v>
+        <v>359</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C137" s="9">
+        <v>5</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="E137" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C138" s="5">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C138" s="9">
+        <v>25</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="E138" s="1"/>
+        <v>318</v>
+      </c>
+      <c r="E138" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="F138" s="1"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="C139" s="9">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C139" s="5">
+        <v>22</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E139" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F139" s="6" t="s">
-        <v>308</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="C140" s="9">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C140" s="5">
+        <v>54</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="E140" s="6" t="s">
-        <v>309</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="E140" s="1"/>
       <c r="F140" s="1"/>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B141" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="C141" s="9">
-        <v>76</v>
-      </c>
-      <c r="D141" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="E141" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="F141" s="1"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="C142" s="9">
-        <v>5</v>
-      </c>
-      <c r="D142" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="E142" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F142" s="1"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="C143" s="9">
-        <v>25</v>
-      </c>
-      <c r="D143" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="E143" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="F143" s="1"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C144" s="5">
-        <v>22</v>
-      </c>
-      <c r="D144" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E144" s="1"/>
-      <c r="F144" s="1"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C145" s="5">
-        <v>40</v>
-      </c>
-      <c r="D145" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E145" s="1"/>
-      <c r="F145" s="1"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C146" s="5">
-        <v>54</v>
-      </c>
-      <c r="D146" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E146" s="1"/>
-      <c r="F146" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -10186,7 +10084,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10612,7 +10510,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel e web com celulas em merge. Falta corrigir o warning de celula nao ser serializable e o bug dos horarios shiftados
</commit_message>
<xml_diff>
--- a/excel_sistema.xlsx
+++ b/excel_sistema.xlsx
@@ -1361,15 +1361,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2672,8 +2672,8 @@
         <v>4</v>
       </c>
       <c r="D28" s="18"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
       <c r="G28" s="45"/>
       <c r="H28" s="22"/>
       <c r="I28" s="14"/>
@@ -2681,12 +2681,12 @@
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
-      <c r="N28" s="44"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="18"/>
-      <c r="P28" s="44"/>
+      <c r="P28" s="46"/>
       <c r="Q28" s="18"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="44"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
       <c r="T28" s="45"/>
       <c r="U28" s="22"/>
     </row>
@@ -6976,10 +6976,10 @@
     </row>
     <row r="197" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B197" s="18"/>
-      <c r="C197" s="44"/>
+      <c r="C197" s="46"/>
       <c r="D197" s="18"/>
-      <c r="E197" s="44"/>
-      <c r="F197" s="44"/>
+      <c r="E197" s="46"/>
+      <c r="F197" s="46"/>
       <c r="G197" s="45"/>
       <c r="H197" s="17"/>
       <c r="I197" s="14"/>
@@ -6987,12 +6987,12 @@
       <c r="K197" s="14"/>
       <c r="L197" s="14"/>
       <c r="M197" s="14"/>
-      <c r="N197" s="44"/>
+      <c r="N197" s="46"/>
       <c r="O197" s="18"/>
-      <c r="P197" s="44"/>
+      <c r="P197" s="46"/>
       <c r="Q197" s="18"/>
-      <c r="R197" s="44"/>
-      <c r="S197" s="44"/>
+      <c r="R197" s="46"/>
+      <c r="S197" s="46"/>
       <c r="T197" s="45"/>
       <c r="U197" s="17"/>
     </row>
@@ -7020,12 +7020,12 @@
     </row>
     <row r="199" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B199" s="24"/>
-      <c r="C199" s="44"/>
+      <c r="C199" s="46"/>
       <c r="D199" s="18"/>
-      <c r="E199" s="44"/>
-      <c r="F199" s="44"/>
+      <c r="E199" s="46"/>
+      <c r="F199" s="46"/>
       <c r="G199" s="45"/>
-      <c r="H199" s="46"/>
+      <c r="H199" s="44"/>
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
       <c r="K199" s="14"/>
@@ -7033,12 +7033,12 @@
       <c r="M199" s="14"/>
       <c r="N199" s="47"/>
       <c r="O199" s="24"/>
-      <c r="P199" s="44"/>
+      <c r="P199" s="46"/>
       <c r="Q199" s="18"/>
-      <c r="R199" s="44"/>
-      <c r="S199" s="44"/>
+      <c r="R199" s="46"/>
+      <c r="S199" s="46"/>
       <c r="T199" s="45"/>
-      <c r="U199" s="46"/>
+      <c r="U199" s="44"/>
     </row>
     <row r="200" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B200" s="25"/>
@@ -7460,23 +7460,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="U199:U201"/>
-    <mergeCell ref="N197:N198"/>
-    <mergeCell ref="P197:P198"/>
-    <mergeCell ref="R197:R198"/>
-    <mergeCell ref="S197:S198"/>
-    <mergeCell ref="T197:T198"/>
-    <mergeCell ref="N199:N201"/>
-    <mergeCell ref="P199:P201"/>
-    <mergeCell ref="R199:R201"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="E197:E198"/>
-    <mergeCell ref="F197:F198"/>
-    <mergeCell ref="G197:G198"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="E199:E201"/>
-    <mergeCell ref="F199:F201"/>
-    <mergeCell ref="G199:G201"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
@@ -7488,6 +7471,23 @@
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
     <mergeCell ref="T199:T201"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="E197:E198"/>
+    <mergeCell ref="F197:F198"/>
+    <mergeCell ref="G197:G198"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="E199:E201"/>
+    <mergeCell ref="F199:F201"/>
+    <mergeCell ref="G199:G201"/>
+    <mergeCell ref="U199:U201"/>
+    <mergeCell ref="N197:N198"/>
+    <mergeCell ref="P197:P198"/>
+    <mergeCell ref="R197:R198"/>
+    <mergeCell ref="S197:S198"/>
+    <mergeCell ref="T197:T198"/>
+    <mergeCell ref="N199:N201"/>
+    <mergeCell ref="P199:P201"/>
+    <mergeCell ref="R199:R201"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
@@ -7644,7 +7644,7 @@
   <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140:XFD140"/>
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bug dos horarios corrigido.
</commit_message>
<xml_diff>
--- a/excel_sistema.xlsx
+++ b/excel_sistema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="22995" windowHeight="9975" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="22995" windowHeight="9975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CursoAno" sheetId="1" r:id="rId1"/>
@@ -1360,16 +1360,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1377,6 +1376,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1681,7 +1683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -2119,7 +2121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U218"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
@@ -2672,22 +2674,22 @@
         <v>4</v>
       </c>
       <c r="D28" s="18"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="45"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
       <c r="H28" s="22"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
-      <c r="N28" s="46"/>
+      <c r="N28" s="43"/>
       <c r="O28" s="18"/>
-      <c r="P28" s="46"/>
+      <c r="P28" s="43"/>
       <c r="Q28" s="18"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="45"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="44"/>
       <c r="U28" s="22"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -2701,22 +2703,22 @@
         <v>4</v>
       </c>
       <c r="D29" s="19"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
       <c r="H29" s="21"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
-      <c r="N29" s="45"/>
+      <c r="N29" s="44"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="45"/>
+      <c r="P29" s="44"/>
       <c r="Q29" s="19"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
       <c r="U29" s="21"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -6976,113 +6978,113 @@
     </row>
     <row r="197" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B197" s="18"/>
-      <c r="C197" s="46"/>
+      <c r="C197" s="43"/>
       <c r="D197" s="18"/>
-      <c r="E197" s="46"/>
-      <c r="F197" s="46"/>
-      <c r="G197" s="45"/>
+      <c r="E197" s="43"/>
+      <c r="F197" s="43"/>
+      <c r="G197" s="44"/>
       <c r="H197" s="17"/>
       <c r="I197" s="14"/>
       <c r="J197" s="14"/>
       <c r="K197" s="14"/>
       <c r="L197" s="14"/>
       <c r="M197" s="14"/>
-      <c r="N197" s="46"/>
+      <c r="N197" s="43"/>
       <c r="O197" s="18"/>
-      <c r="P197" s="46"/>
+      <c r="P197" s="43"/>
       <c r="Q197" s="18"/>
-      <c r="R197" s="46"/>
-      <c r="S197" s="46"/>
-      <c r="T197" s="45"/>
+      <c r="R197" s="43"/>
+      <c r="S197" s="43"/>
+      <c r="T197" s="44"/>
       <c r="U197" s="17"/>
     </row>
     <row r="198" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B198" s="19"/>
-      <c r="C198" s="45"/>
+      <c r="C198" s="44"/>
       <c r="D198" s="19"/>
-      <c r="E198" s="45"/>
-      <c r="F198" s="45"/>
-      <c r="G198" s="45"/>
+      <c r="E198" s="44"/>
+      <c r="F198" s="44"/>
+      <c r="G198" s="44"/>
       <c r="H198" s="17"/>
       <c r="I198" s="14"/>
       <c r="J198" s="14"/>
       <c r="K198" s="14"/>
       <c r="L198" s="14"/>
       <c r="M198" s="14"/>
-      <c r="N198" s="45"/>
+      <c r="N198" s="44"/>
       <c r="O198" s="19"/>
-      <c r="P198" s="45"/>
+      <c r="P198" s="44"/>
       <c r="Q198" s="19"/>
-      <c r="R198" s="45"/>
-      <c r="S198" s="45"/>
-      <c r="T198" s="45"/>
+      <c r="R198" s="44"/>
+      <c r="S198" s="44"/>
+      <c r="T198" s="44"/>
       <c r="U198" s="17"/>
     </row>
     <row r="199" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B199" s="24"/>
-      <c r="C199" s="46"/>
+      <c r="C199" s="43"/>
       <c r="D199" s="18"/>
-      <c r="E199" s="46"/>
-      <c r="F199" s="46"/>
-      <c r="G199" s="45"/>
-      <c r="H199" s="44"/>
+      <c r="E199" s="43"/>
+      <c r="F199" s="43"/>
+      <c r="G199" s="44"/>
+      <c r="H199" s="45"/>
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
       <c r="K199" s="14"/>
       <c r="L199" s="14"/>
       <c r="M199" s="14"/>
-      <c r="N199" s="47"/>
+      <c r="N199" s="46"/>
       <c r="O199" s="24"/>
-      <c r="P199" s="46"/>
+      <c r="P199" s="43"/>
       <c r="Q199" s="18"/>
-      <c r="R199" s="46"/>
-      <c r="S199" s="46"/>
-      <c r="T199" s="45"/>
-      <c r="U199" s="44"/>
+      <c r="R199" s="43"/>
+      <c r="S199" s="43"/>
+      <c r="T199" s="44"/>
+      <c r="U199" s="45"/>
     </row>
     <row r="200" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B200" s="25"/>
-      <c r="C200" s="45"/>
+      <c r="C200" s="44"/>
       <c r="D200" s="19"/>
-      <c r="E200" s="45"/>
-      <c r="F200" s="45"/>
-      <c r="G200" s="45"/>
-      <c r="H200" s="45"/>
+      <c r="E200" s="44"/>
+      <c r="F200" s="44"/>
+      <c r="G200" s="44"/>
+      <c r="H200" s="44"/>
       <c r="I200" s="14"/>
       <c r="J200" s="14"/>
       <c r="K200" s="14"/>
       <c r="L200" s="14"/>
       <c r="M200" s="14"/>
-      <c r="N200" s="48"/>
+      <c r="N200" s="47"/>
       <c r="O200" s="25"/>
-      <c r="P200" s="45"/>
+      <c r="P200" s="44"/>
       <c r="Q200" s="19"/>
-      <c r="R200" s="45"/>
-      <c r="S200" s="45"/>
-      <c r="T200" s="45"/>
-      <c r="U200" s="45"/>
+      <c r="R200" s="44"/>
+      <c r="S200" s="44"/>
+      <c r="T200" s="44"/>
+      <c r="U200" s="44"/>
     </row>
     <row r="201" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B201" s="25"/>
-      <c r="C201" s="45"/>
+      <c r="C201" s="44"/>
       <c r="D201" s="19"/>
-      <c r="E201" s="45"/>
-      <c r="F201" s="45"/>
-      <c r="G201" s="45"/>
-      <c r="H201" s="45"/>
+      <c r="E201" s="44"/>
+      <c r="F201" s="44"/>
+      <c r="G201" s="44"/>
+      <c r="H201" s="44"/>
       <c r="I201" s="14"/>
       <c r="J201" s="14"/>
       <c r="K201" s="14"/>
       <c r="L201" s="14"/>
       <c r="M201" s="14"/>
-      <c r="N201" s="48"/>
+      <c r="N201" s="47"/>
       <c r="O201" s="25"/>
-      <c r="P201" s="45"/>
+      <c r="P201" s="44"/>
       <c r="Q201" s="19"/>
-      <c r="R201" s="45"/>
-      <c r="S201" s="45"/>
-      <c r="T201" s="45"/>
-      <c r="U201" s="45"/>
+      <c r="R201" s="44"/>
+      <c r="S201" s="44"/>
+      <c r="T201" s="44"/>
+      <c r="U201" s="44"/>
     </row>
     <row r="202" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B202" s="12"/>
@@ -7460,6 +7462,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="U199:U201"/>
+    <mergeCell ref="N197:N198"/>
+    <mergeCell ref="P197:P198"/>
+    <mergeCell ref="R197:R198"/>
+    <mergeCell ref="S197:S198"/>
+    <mergeCell ref="T197:T198"/>
+    <mergeCell ref="N199:N201"/>
+    <mergeCell ref="P199:P201"/>
+    <mergeCell ref="R199:R201"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="E197:E198"/>
+    <mergeCell ref="F197:F198"/>
+    <mergeCell ref="G197:G198"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="E199:E201"/>
+    <mergeCell ref="F199:F201"/>
+    <mergeCell ref="G199:G201"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
@@ -7471,23 +7490,6 @@
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
     <mergeCell ref="T199:T201"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="E197:E198"/>
-    <mergeCell ref="F197:F198"/>
-    <mergeCell ref="G197:G198"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="E199:E201"/>
-    <mergeCell ref="F199:F201"/>
-    <mergeCell ref="G199:G201"/>
-    <mergeCell ref="U199:U201"/>
-    <mergeCell ref="N197:N198"/>
-    <mergeCell ref="P197:P198"/>
-    <mergeCell ref="R197:R198"/>
-    <mergeCell ref="S197:S198"/>
-    <mergeCell ref="T197:T198"/>
-    <mergeCell ref="N199:N201"/>
-    <mergeCell ref="P199:P201"/>
-    <mergeCell ref="R199:R201"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
@@ -7496,10 +7498,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7530,39 +7532,37 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>0.4236111111111111</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.49305555555555558</v>
-      </c>
+        <v>0.375</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>0.46527777777777773</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="B5" s="4">
-        <v>0.5</v>
+        <v>0.49305555555555558</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="B6" s="4">
         <v>0.5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="4">
         <v>0.55555555555555558</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>0.59722222222222221</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="B8" s="4">
         <v>0.66666666666666663</v>
@@ -7570,68 +7570,78 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>0.63194444444444442</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="B9" s="4">
-        <v>0.68055555555555547</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="B10" s="4">
         <v>0.68055555555555547</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0.79166666666666663</v>
-      </c>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="B13" s="4">
         <v>0.79166666666666663</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B14" s="4">
         <v>0.83333333333333337</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.875</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B15" s="4">
         <v>0.875</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="B16" s="4">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="48">
+        <v>0.94444444444444453</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7643,8 +7653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>